<commit_message>
Allow all plant types to be built for reliability and set dispatch cost multiplier to 1 (#232)
</commit_message>
<xml_diff>
--- a/InputData/elec/BPTBfRN/Boolean Plant Types Built for Reliability Needs.xlsx
+++ b/InputData/elec/BPTBfRN/Boolean Plant Types Built for Reliability Needs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\BPTBfRN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E6A413-A824-425A-89D8-3C918CDD1061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C398B7-2F93-4ADF-8C9E-E281EEC55201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4755" yWindow="6645" windowWidth="29505" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="2025" windowWidth="19710" windowHeight="20325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -572,7 +572,7 @@
         <v>13</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -580,7 +580,7 @@
         <v>19</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -588,7 +588,7 @@
         <v>20</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -596,7 +596,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -604,7 +604,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -620,7 +620,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -628,7 +628,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -636,7 +636,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -644,7 +644,7 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -669,7 +669,7 @@
       </c>
       <c r="B14">
         <f>B2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -678,7 +678,7 @@
       </c>
       <c r="B15">
         <f>B7</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -703,7 +703,7 @@
       </c>
       <c r="B18">
         <f>B10</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calibration based data updates.
</commit_message>
<xml_diff>
--- a/InputData/elec/BPTBfRN/Boolean Plant Types Built for Reliability Needs.xlsx
+++ b/InputData/elec/BPTBfRN/Boolean Plant Types Built for Reliability Needs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\BPTBfRN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\BPTBfRN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FC3A9D-6F7F-4527-A818-85FD4D4CFA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80DAE91-F84C-4936-939C-09AE56C5F154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="3330" windowWidth="28770" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -484,7 +484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -539,8 +539,8 @@
   </sheetPr>
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>